<commit_message>
add 'clean' versions of queries in English
</commit_message>
<xml_diff>
--- a/retrieval/Translated Query.xlsx
+++ b/retrieval/Translated Query.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="630" yWindow="570" windowWidth="26535" windowHeight="11700" activeTab="2"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Chinese" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Arabic" sheetId="2" r:id="rId4"/>
+    <sheet name="Chinese" sheetId="1" r:id="rId1"/>
+    <sheet name="Arabic" sheetId="2" r:id="rId2"/>
+    <sheet name="English" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="154">
   <si>
     <t>ID</t>
   </si>
@@ -324,32 +328,191 @@
   </si>
   <si>
     <t>عندما نحن أسعد؟ يمكننا أن تصبح أكثر سعادة؟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harmful effects of video games </t>
+  </si>
+  <si>
+    <t>Is it harmful to play video games Does playing make people violent Does it damage attention spans Does it increase obesity Are people who play video games less fit Should video games be banned"</t>
+  </si>
+  <si>
+    <t>Do cycle lanes increase or decrease congestion and pollution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bike lanes and congestion and pollution </t>
+  </si>
+  <si>
+    <t>What are good study habits How common are they Is it better to study a little every day or focus for a concentrated period of time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good study habits </t>
+  </si>
+  <si>
+    <t>How can we save energy in our daily lives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how to save energy at home </t>
+  </si>
+  <si>
+    <t>Why are we so ignorant about the world</t>
+  </si>
+  <si>
+    <t xml:space="preserve">human ignorance </t>
+  </si>
+  <si>
+    <t>How can music affect our body mind Does music changes our emotions or attitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impact of music </t>
+  </si>
+  <si>
+    <t>Why do we procrastinate How can we avoid procrastinating on important task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procrastination </t>
+  </si>
+  <si>
+    <t>What are the evidence that points to climate change is it a hoax what can we do to slow it down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">climate change </t>
+  </si>
+  <si>
+    <t>What are the pros and cons of implementing basic income scheme in a country What are some of the preliminary results for countries states that have implemented such scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">basic income </t>
+  </si>
+  <si>
+    <t>Does Artificial Intelligence smarter than human Can AI replace the brain of human being To what extent the field of AI can affect the people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artificial intelligence smarter than human </t>
+  </si>
+  <si>
+    <t>The meaning of doodles and how Psychologists can use it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doodlers behavior </t>
+  </si>
+  <si>
+    <t>What is IoT and the current concerns about IoT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internet of things evolution </t>
+  </si>
+  <si>
+    <t>Can women be leader Do women can do things the men could not What makes women strong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The power of women </t>
+  </si>
+  <si>
+    <t>How does classical music affect us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effect of classical music </t>
+  </si>
+  <si>
+    <t>How does body language affects how others see us and how can it also change how we see ourselves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">importance of body language </t>
+  </si>
+  <si>
+    <t>Why creating an education system that nurtures rather than undermines creativity is important</t>
+  </si>
+  <si>
+    <t xml:space="preserve">importance of creativity in schools </t>
+  </si>
+  <si>
+    <t>How to avoid making critical mistakes in stressful situations when your thinking becomes clouded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how to stay calm </t>
+  </si>
+  <si>
+    <t>How to stay motivated when doing different tasks even if you have lost interest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how to stay motivated </t>
+  </si>
+  <si>
+    <t>What are the cutest animals and what makes them cute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cute animals </t>
+  </si>
+  <si>
+    <t>what are the psychological or sociological effects of social media on us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effects of social media </t>
+  </si>
+  <si>
+    <t>what determines if something is art and if it is good art</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what is art </t>
+  </si>
+  <si>
+    <t>What qualifies as being disabled Are we cognizant of the needs of everyone around us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disability </t>
+  </si>
+  <si>
+    <t>Which areas are most affected Why is extremism rising and how to build a safer society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rise of terrorism </t>
+  </si>
+  <si>
+    <t>How did the universe start Are we real and why is the world the way we see it is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">why do we exist </t>
+  </si>
+  <si>
+    <t>When are we the happiest Can we become happier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secret to happiness </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -357,7 +520,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -367,77 +530,370 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="21.14"/>
-    <col customWidth="1" min="4" max="4" width="52.0"/>
-    <col customWidth="1" min="5" max="5" width="40.57"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="52" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,12 +908,12 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="B2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
@@ -467,12 +923,12 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
@@ -482,12 +938,12 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -497,12 +953,12 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="B5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>16</v>
@@ -512,12 +968,12 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="B6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>20</v>
@@ -527,12 +983,12 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <v>202.0</v>
+        <v>202</v>
       </c>
       <c r="B7" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -542,12 +998,12 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>203.0</v>
+        <v>203</v>
       </c>
       <c r="B8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>30</v>
@@ -557,12 +1013,12 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>204.0</v>
+        <v>204</v>
       </c>
       <c r="B9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>34</v>
@@ -572,12 +1028,12 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>205.0</v>
+        <v>205</v>
       </c>
       <c r="B10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>38</v>
@@ -587,12 +1043,12 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>301.0</v>
+        <v>301</v>
       </c>
       <c r="B11" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>42</v>
@@ -602,12 +1058,12 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <v>302.0</v>
+        <v>302</v>
       </c>
       <c r="B12" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>46</v>
@@ -617,12 +1073,12 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <v>303.0</v>
+        <v>303</v>
       </c>
       <c r="B13" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>49</v>
@@ -632,12 +1088,12 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>304.0</v>
+        <v>304</v>
       </c>
       <c r="B14" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>53</v>
@@ -647,12 +1103,12 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <v>305.0</v>
+        <v>305</v>
       </c>
       <c r="B15" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>56</v>
@@ -662,12 +1118,12 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <v>306.0</v>
+        <v>306</v>
       </c>
       <c r="B16" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>60</v>
@@ -677,12 +1133,12 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <v>307.0</v>
+        <v>307</v>
       </c>
       <c r="B17" s="3">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>63</v>
@@ -692,12 +1148,12 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <v>308.0</v>
+        <v>308</v>
       </c>
       <c r="B18" s="3">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>65</v>
@@ -707,12 +1163,12 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <v>401.0</v>
+        <v>401</v>
       </c>
       <c r="B19" s="3">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>67</v>
@@ -722,12 +1178,12 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
-        <v>402.0</v>
+        <v>402</v>
       </c>
       <c r="B20" s="3">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>69</v>
@@ -737,12 +1193,12 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <v>403.0</v>
+        <v>403</v>
       </c>
       <c r="B21" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>71</v>
@@ -752,12 +1208,12 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
-        <v>404.0</v>
+        <v>404</v>
       </c>
       <c r="B22" s="3">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>73</v>
@@ -767,12 +1223,12 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
-        <v>501.0</v>
+        <v>501</v>
       </c>
       <c r="B23" s="3">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>75</v>
@@ -782,12 +1238,12 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <v>502.0</v>
+        <v>502</v>
       </c>
       <c r="B24" s="3">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>77</v>
@@ -797,12 +1253,12 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
-        <v>503.0</v>
+        <v>503</v>
       </c>
       <c r="B25" s="3">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>80</v>
@@ -812,12 +1268,12 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
-        <v>504.0</v>
+        <v>504</v>
       </c>
       <c r="B26" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>82</v>
@@ -828,22 +1284,23 @@
       <c r="E26" s="7"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="24.29"/>
-    <col customWidth="1" min="4" max="6" width="58.43"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="6" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -859,12 +1316,12 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="B2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -875,12 +1332,12 @@
       <c r="E2" s="6"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -891,12 +1348,12 @@
       <c r="E3" s="6"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>13</v>
@@ -907,12 +1364,12 @@
       <c r="E4" s="6"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="B5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>17</v>
@@ -923,12 +1380,12 @@
       <c r="E5" s="6"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="B6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>22</v>
@@ -939,12 +1396,12 @@
       <c r="E6" s="6"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <v>202.0</v>
+        <v>202</v>
       </c>
       <c r="B7" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>26</v>
@@ -955,12 +1412,12 @@
       <c r="E7" s="6"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>203.0</v>
+        <v>203</v>
       </c>
       <c r="B8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>28</v>
@@ -971,12 +1428,12 @@
       <c r="E8" s="6"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>204.0</v>
+        <v>204</v>
       </c>
       <c r="B9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>31</v>
@@ -987,12 +1444,12 @@
       <c r="E9" s="6"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>205.0</v>
+        <v>205</v>
       </c>
       <c r="B10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>36</v>
@@ -1003,12 +1460,12 @@
       <c r="E10" s="6"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>301.0</v>
+        <v>301</v>
       </c>
       <c r="B11" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>40</v>
@@ -1019,12 +1476,12 @@
       <c r="E11" s="6"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <v>302.0</v>
+        <v>302</v>
       </c>
       <c r="B12" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>44</v>
@@ -1035,12 +1492,12 @@
       <c r="E12" s="6"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <v>303.0</v>
+        <v>303</v>
       </c>
       <c r="B13" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>48</v>
@@ -1051,12 +1508,12 @@
       <c r="E13" s="6"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>304.0</v>
+        <v>304</v>
       </c>
       <c r="B14" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>52</v>
@@ -1067,12 +1524,12 @@
       <c r="E14" s="6"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <v>305.0</v>
+        <v>305</v>
       </c>
       <c r="B15" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>57</v>
@@ -1083,12 +1540,12 @@
       <c r="E15" s="6"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <v>306.0</v>
+        <v>306</v>
       </c>
       <c r="B16" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>61</v>
@@ -1099,12 +1556,12 @@
       <c r="E16" s="6"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <v>307.0</v>
+        <v>307</v>
       </c>
       <c r="B17" s="3">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>84</v>
@@ -1115,12 +1572,12 @@
       <c r="E17" s="6"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <v>308.0</v>
+        <v>308</v>
       </c>
       <c r="B18" s="3">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>86</v>
@@ -1131,12 +1588,12 @@
       <c r="E18" s="6"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <v>401.0</v>
+        <v>401</v>
       </c>
       <c r="B19" s="3">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>88</v>
@@ -1147,12 +1604,12 @@
       <c r="E19" s="6"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
-        <v>402.0</v>
+        <v>402</v>
       </c>
       <c r="B20" s="3">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>90</v>
@@ -1163,12 +1620,12 @@
       <c r="E20" s="6"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <v>403.0</v>
+        <v>403</v>
       </c>
       <c r="B21" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>92</v>
@@ -1179,12 +1636,12 @@
       <c r="E21" s="6"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
-        <v>404.0</v>
+        <v>404</v>
       </c>
       <c r="B22" s="3">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>94</v>
@@ -1195,12 +1652,12 @@
       <c r="E22" s="6"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
-        <v>501.0</v>
+        <v>501</v>
       </c>
       <c r="B23" s="3">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>96</v>
@@ -1211,12 +1668,12 @@
       <c r="E23" s="6"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <v>502.0</v>
+        <v>502</v>
       </c>
       <c r="B24" s="3">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>98</v>
@@ -1227,12 +1684,12 @@
       <c r="E24" s="6"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
-        <v>503.0</v>
+        <v>503</v>
       </c>
       <c r="B25" s="3">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>100</v>
@@ -1243,12 +1700,12 @@
       <c r="E25" s="6"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
-        <v>504.0</v>
+        <v>504</v>
       </c>
       <c r="B26" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>102</v>
@@ -1260,6 +1717,419 @@
       <c r="F26" s="8"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>101</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>102</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>103</v>
+      </c>
+      <c r="B4" s="14">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>104</v>
+      </c>
+      <c r="B5" s="14">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>201</v>
+      </c>
+      <c r="B6" s="14">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>202</v>
+      </c>
+      <c r="B7" s="14">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>203</v>
+      </c>
+      <c r="B8" s="14">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>204</v>
+      </c>
+      <c r="B9" s="14">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>205</v>
+      </c>
+      <c r="B10" s="14">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <v>301</v>
+      </c>
+      <c r="B11" s="14">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14">
+        <v>302</v>
+      </c>
+      <c r="B12" s="14">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
+        <v>303</v>
+      </c>
+      <c r="B13" s="14">
+        <v>12</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>304</v>
+      </c>
+      <c r="B14" s="14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
+        <v>305</v>
+      </c>
+      <c r="B15" s="14">
+        <v>14</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14">
+        <v>306</v>
+      </c>
+      <c r="B16" s="14">
+        <v>15</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14">
+        <v>307</v>
+      </c>
+      <c r="B17" s="14">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14">
+        <v>308</v>
+      </c>
+      <c r="B18" s="14">
+        <v>17</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
+        <v>401</v>
+      </c>
+      <c r="B19" s="14">
+        <v>18</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14">
+        <v>402</v>
+      </c>
+      <c r="B20" s="14">
+        <v>19</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14">
+        <v>403</v>
+      </c>
+      <c r="B21" s="14">
+        <v>20</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14">
+        <v>404</v>
+      </c>
+      <c r="B22" s="14">
+        <v>21</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14">
+        <v>501</v>
+      </c>
+      <c r="B23" s="14">
+        <v>22</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14">
+        <v>502</v>
+      </c>
+      <c r="B24" s="14">
+        <v>23</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14">
+        <v>503</v>
+      </c>
+      <c r="B25" s="14">
+        <v>24</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14">
+        <v>504</v>
+      </c>
+      <c r="B26" s="14">
+        <v>25</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated: Wei Ting checked + Cleaned Translated Queries
</commit_message>
<xml_diff>
--- a/retrieval/Translated Query.xlsx
+++ b/retrieval/Translated Query.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chinese" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,100 +36,73 @@
     <t xml:space="preserve">desc</t>
   </si>
   <si>
-    <t xml:space="preserve">视频游戏有害影响</t>
-  </si>
-  <si>
-    <t xml:space="preserve">它是有害的玩视频游戏播放是否让人暴力是否损坏的注意力是否增加肥胖是谁玩视频游戏不太适合视频是否应进行游戏禁止人</t>
+    <t xml:space="preserve">视频游戏的害影响</t>
+  </si>
+  <si>
+    <t xml:space="preserve">玩视频游戏是否有害处 玩视频游戏会让人暴力吗 它是否损坏的注意力 是否增加肥胖 玩视频电影会让损害身体吗 视频游戏应该被禁止吗</t>
   </si>
   <si>
     <t xml:space="preserve">自行车道和拥堵和污染</t>
   </si>
   <si>
-    <t xml:space="preserve">做自行车道增加或减少拥堵和污染</t>
+    <t xml:space="preserve">自行车道增加或减少拥堵和污染</t>
   </si>
   <si>
     <t xml:space="preserve">良好的学习习惯</t>
   </si>
   <si>
-    <t xml:space="preserve">什么是良好的学习习惯如何常见的是，他们是更好每天学习一点或集中的时间集中的时期</t>
+    <t xml:space="preserve">什么是良好的学习习惯 他们是否常见 更好每天学习一点 或集中的时间集中的时期</t>
   </si>
   <si>
     <t xml:space="preserve">如何节约能源在家里</t>
   </si>
   <si>
-    <t xml:space="preserve">我们怎样才能节约能源在我们的日常生活</t>
+    <t xml:space="preserve">我们怎样才能在我们的日常生活中节约能源</t>
   </si>
   <si>
     <t xml:space="preserve">人类的无知</t>
   </si>
   <si>
-    <t xml:space="preserve">为什么我们这么无知的世界</t>
+    <t xml:space="preserve">为什么我们这么无知</t>
   </si>
   <si>
     <t xml:space="preserve">音乐的影响</t>
   </si>
   <si>
-    <t xml:space="preserve">如何音乐影响我们的身体心灵的音乐是否改变我们的情绪或态度</t>
+    <t xml:space="preserve">音乐如何影响我们的身体和心灵 音乐是否改变我们的情绪和态度</t>
   </si>
   <si>
     <t xml:space="preserve">拖延</t>
   </si>
   <si>
-    <t xml:space="preserve">我们为什么要拖延，我们怎样才能避免拖延的重要任务</t>
+    <t xml:space="preserve">我们为什么要拖延 我们怎样才能避免拖延重要的任务</t>
   </si>
   <si>
     <t xml:space="preserve">气候变化</t>
   </si>
   <si>
-    <t xml:space="preserve">什么是指向气候变化的证据，它是一个骗局，我们能做些什么来慢下来</t>
+    <t xml:space="preserve">什么证据指向气候变化 它是一个骗局吗 我们能做些什么才能让它慢下来</t>
   </si>
   <si>
     <t xml:space="preserve">基本收入</t>
   </si>
   <si>
-    <t xml:space="preserve">什么是什么是一些已经实施这种方案的国家状态的初步结果的执行在一个国家基本收入计划的利弊</t>
+    <t xml:space="preserve">实行基本收入有什么利弊 已经实施这种方案的国家有什么初步的结果</t>
   </si>
   <si>
     <t xml:space="preserve">人工智能比人类更聪明</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">是否人工智能比人类更聪明的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">AI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">能代替人类的大脑在多大程度上人工智能领域可以影响人</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">为涂鸦行为</t>
-  </si>
-  <si>
-    <t xml:space="preserve">涂鸦的意义，以及如何心理学家可以用它</t>
-  </si>
-  <si>
-    <t xml:space="preserve">事情演变的互联网</t>
+    <t xml:space="preserve">人工智能是否比人类聪明 人工智能可取代人脑吗 人工智能领域在什么程度上影响人类</t>
+  </si>
+  <si>
+    <t xml:space="preserve">为涂鸦的行为</t>
+  </si>
+  <si>
+    <t xml:space="preserve">涂鸦的意义 心理学家如何利用涂鸦</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 物联网的进化</t>
   </si>
   <si>
     <t xml:space="preserve">什么是物联网与物联网有关当前关注</t>
@@ -138,46 +111,46 @@
     <t xml:space="preserve">女人的力量</t>
   </si>
   <si>
-    <t xml:space="preserve">女性可以领导做女人可以做的事情的人不能是什么让女人强</t>
+    <t xml:space="preserve">女性可以领导吗 女人可以做男人不能做的事情吗 是什么让女人强</t>
   </si>
   <si>
     <t xml:space="preserve">古典音乐的影响</t>
   </si>
   <si>
-    <t xml:space="preserve">如何古典音乐影响我们</t>
+    <t xml:space="preserve">古典音如何乐影响我们</t>
   </si>
   <si>
     <t xml:space="preserve">身体语言的重要性</t>
   </si>
   <si>
-    <t xml:space="preserve">如何肢体语言会影响别人怎么看我们，怎么也可以改变我们看待自己</t>
+    <t xml:space="preserve">肢体语言如何影响别人对我们的观点和 和改变我们如何看待自己</t>
   </si>
   <si>
     <t xml:space="preserve">在学校创造力的重要性</t>
   </si>
   <si>
-    <t xml:space="preserve">为什么要创建一个教育体系培育，而不是破坏的创意是非常重要的</t>
+    <t xml:space="preserve">为什么要创建一个培育创新 而不是压抑 的教育系统是非常重要的</t>
   </si>
   <si>
     <t xml:space="preserve">如何保持冷静</t>
   </si>
   <si>
-    <t xml:space="preserve">如何避免在紧张的情况下做出重要的错误时，你的思维变得乌云密布</t>
+    <t xml:space="preserve">如何避免在紧张的情况下做出重要的错误</t>
   </si>
   <si>
     <t xml:space="preserve">如何保持动力</t>
   </si>
   <si>
-    <t xml:space="preserve">如何做不同的任务时，即使你已经失去了兴趣，保持动力</t>
+    <t xml:space="preserve">如何做不同的任务时 即使你已经失去了兴趣 保持动力</t>
   </si>
   <si>
     <t xml:space="preserve">可爱的动物</t>
   </si>
   <si>
-    <t xml:space="preserve">什么是最可爱的动物，是什么让他们可爱</t>
-  </si>
-  <si>
-    <t xml:space="preserve">社会化媒体的影响</t>
+    <t xml:space="preserve">什么是最可爱的动物 是什么让他们可爱</t>
+  </si>
+  <si>
+    <t xml:space="preserve">社交化媒体的影响</t>
   </si>
   <si>
     <t xml:space="preserve">什么是社交媒体对我们的心理和社会学的影响</t>
@@ -186,31 +159,31 @@
     <t xml:space="preserve">什么是艺术</t>
   </si>
   <si>
-    <t xml:space="preserve">是什么决定了，如果事情是艺术，如果是好的艺术</t>
+    <t xml:space="preserve">是什么决定艺术 和好的艺术</t>
   </si>
   <si>
     <t xml:space="preserve">失能</t>
   </si>
   <si>
-    <t xml:space="preserve">有什么资格成为被禁用的，我们认识到每个人的身边需要</t>
+    <t xml:space="preserve">列为残疾人士的标准是什么 我们是否意思到周遭认识的需求</t>
   </si>
   <si>
     <t xml:space="preserve">恐怖主义的崛起</t>
   </si>
   <si>
-    <t xml:space="preserve">哪些地区受影响最严重为什么极端主义上升，以及如何建立一个更安全的社会</t>
+    <t xml:space="preserve">哪些地区受到被恐怖主义的影响最大 为什么极端主义有上升的趋势 我们如何建立一个更安全的社会呢</t>
   </si>
   <si>
     <t xml:space="preserve">为什么我们存在</t>
   </si>
   <si>
-    <t xml:space="preserve">宇宙是如何开始我们是真实的，为什么是世界上我们所看到的事情是这样的</t>
-  </si>
-  <si>
-    <t xml:space="preserve">秘密幸福</t>
-  </si>
-  <si>
-    <t xml:space="preserve">当我们是最幸福的，我们能成为快乐</t>
+    <t xml:space="preserve">宇宙是如何开始 我们是真的吗 我们如何领会这个世界</t>
+  </si>
+  <si>
+    <t xml:space="preserve">幸福的秘诀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">我们时候最幸福 我们怎能更幸福呢</t>
   </si>
   <si>
     <t xml:space="preserve">الآثار الضارة للألعاب الفيديو</t>
@@ -603,8 +576,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
     </font>
@@ -670,7 +642,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -688,11 +660,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -735,7 +711,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -979,7 +955,7 @@
       <c r="B16" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -994,7 +970,7 @@
       <c r="B17" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1155,7 +1131,7 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1190,14 +1166,14 @@
       <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="7"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
@@ -1206,14 +1182,14 @@
       <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
@@ -1222,14 +1198,14 @@
       <c r="B4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="7"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -1238,14 +1214,14 @@
       <c r="B5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>61</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="7"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
@@ -1254,14 +1230,14 @@
       <c r="B6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="7"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
@@ -1270,14 +1246,14 @@
       <c r="B7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="7"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
@@ -1286,14 +1262,14 @@
       <c r="B8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="7"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -1302,14 +1278,14 @@
       <c r="B9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="7"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
@@ -1318,14 +1294,14 @@
       <c r="B10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>71</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="7"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
@@ -1334,14 +1310,14 @@
       <c r="B11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
@@ -1350,14 +1326,14 @@
       <c r="B12" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
@@ -1366,14 +1342,14 @@
       <c r="B13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>77</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
@@ -1382,14 +1358,14 @@
       <c r="B14" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>79</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
@@ -1398,14 +1374,14 @@
       <c r="B15" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>81</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="7"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
@@ -1414,14 +1390,14 @@
       <c r="B16" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>83</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
@@ -1430,14 +1406,14 @@
       <c r="B17" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="7" t="s">
         <v>85</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
@@ -1446,14 +1422,14 @@
       <c r="B18" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="8"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
@@ -1462,14 +1438,14 @@
       <c r="B19" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>89</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="8"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
@@ -1478,14 +1454,14 @@
       <c r="B20" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="7"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
@@ -1494,14 +1470,14 @@
       <c r="B21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>93</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="7"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
@@ -1510,14 +1486,14 @@
       <c r="B22" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>95</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="n">
@@ -1526,14 +1502,14 @@
       <c r="B23" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>97</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="8"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="n">
@@ -1542,14 +1518,14 @@
       <c r="B24" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="7" t="s">
         <v>99</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="8"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="n">
@@ -1558,14 +1534,14 @@
       <c r="B25" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>101</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="8"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
@@ -1574,14 +1550,14 @@
       <c r="B26" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="7" t="s">
         <v>103</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1601,7 +1577,7 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1610,7 +1586,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.56122448979592"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="64.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="64.3928571428571"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.0918367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.1734693877551"/>
   </cols>
@@ -1631,376 +1607,376 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="n">
+      <c r="A2" s="11" t="n">
         <v>101</v>
       </c>
-      <c r="B2" s="10" t="n">
+      <c r="B2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>105</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="11" t="n">
         <v>102</v>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>107</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="11" t="n">
         <v>103</v>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>109</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="11" t="n">
         <v>104</v>
       </c>
-      <c r="B5" s="10" t="n">
+      <c r="B5" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>111</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="11" t="n">
         <v>201</v>
       </c>
-      <c r="B6" s="10" t="n">
+      <c r="B6" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>113</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="11" t="n">
         <v>202</v>
       </c>
-      <c r="B7" s="10" t="n">
+      <c r="B7" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>115</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="11" t="n">
         <v>203</v>
       </c>
-      <c r="B8" s="10" t="n">
+      <c r="B8" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>117</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
+      <c r="A9" s="11" t="n">
         <v>204</v>
       </c>
-      <c r="B9" s="10" t="n">
+      <c r="B9" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>119</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="11" t="n">
         <v>205</v>
       </c>
-      <c r="B10" s="10" t="n">
+      <c r="B10" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>121</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="11" t="n">
         <v>301</v>
       </c>
-      <c r="B11" s="10" t="n">
+      <c r="B11" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>123</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="11" t="n">
         <v>302</v>
       </c>
-      <c r="B12" s="10" t="n">
+      <c r="B12" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="8" t="s">
         <v>125</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="11" t="n">
         <v>303</v>
       </c>
-      <c r="B13" s="10" t="n">
+      <c r="B13" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="11" t="n">
         <v>304</v>
       </c>
-      <c r="B14" s="10" t="n">
+      <c r="B14" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="8" t="s">
         <v>129</v>
       </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="n">
+      <c r="A15" s="11" t="n">
         <v>305</v>
       </c>
-      <c r="B15" s="10" t="n">
+      <c r="B15" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="11" t="n">
         <v>306</v>
       </c>
-      <c r="B16" s="10" t="n">
+      <c r="B16" s="11" t="n">
         <v>15</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="8" t="s">
         <v>133</v>
       </c>
       <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="11" t="n">
         <v>307</v>
       </c>
-      <c r="B17" s="10" t="n">
+      <c r="B17" s="11" t="n">
         <v>16</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="8" t="s">
         <v>135</v>
       </c>
       <c r="E17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="n">
+      <c r="A18" s="11" t="n">
         <v>308</v>
       </c>
-      <c r="B18" s="10" t="n">
+      <c r="B18" s="11" t="n">
         <v>17</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="8" t="s">
         <v>137</v>
       </c>
       <c r="E18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="n">
+      <c r="A19" s="11" t="n">
         <v>401</v>
       </c>
-      <c r="B19" s="10" t="n">
+      <c r="B19" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="8" t="s">
         <v>139</v>
       </c>
       <c r="E19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="n">
+      <c r="A20" s="11" t="n">
         <v>402</v>
       </c>
-      <c r="B20" s="10" t="n">
+      <c r="B20" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="8" t="s">
         <v>141</v>
       </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="n">
+      <c r="A21" s="11" t="n">
         <v>403</v>
       </c>
-      <c r="B21" s="10" t="n">
+      <c r="B21" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="8" t="s">
         <v>143</v>
       </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="n">
+      <c r="A22" s="11" t="n">
         <v>404</v>
       </c>
-      <c r="B22" s="10" t="n">
+      <c r="B22" s="11" t="n">
         <v>21</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="8" t="s">
         <v>145</v>
       </c>
       <c r="E22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="n">
+      <c r="A23" s="11" t="n">
         <v>501</v>
       </c>
-      <c r="B23" s="10" t="n">
+      <c r="B23" s="11" t="n">
         <v>22</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="8" t="s">
         <v>147</v>
       </c>
       <c r="E23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="n">
+      <c r="A24" s="11" t="n">
         <v>502</v>
       </c>
-      <c r="B24" s="10" t="n">
+      <c r="B24" s="11" t="n">
         <v>23</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="8" t="s">
         <v>149</v>
       </c>
       <c r="E24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="n">
+      <c r="A25" s="11" t="n">
         <v>503</v>
       </c>
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="11" t="n">
         <v>24</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="8" t="s">
         <v>151</v>
       </c>
       <c r="E25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="n">
+      <c r="A26" s="11" t="n">
         <v>504</v>
       </c>
-      <c r="B26" s="10" t="n">
+      <c r="B26" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="8" t="s">
         <v>153</v>
       </c>
       <c r="E26" s="5"/>

</xml_diff>